<commit_message>
up-to-date documentation and source code added
</commit_message>
<xml_diff>
--- a/schemes/pinouts.xlsx
+++ b/schemes/pinouts.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f92a95b8a3ebd29/Robot/WRO2024/FE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f92a95b8a3ebd29/Dokumentumok/wro2022-fe-template/schemes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{4D398EB6-84DA-43A4-9D8F-54E6CE081F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6160122F-58F1-40F7-A1B7-BF5C7479DA64}"/>
+  <xr:revisionPtr revIDLastSave="377" documentId="8_{4D398EB6-84DA-43A4-9D8F-54E6CE081F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B780DF9-F16E-453A-AFE5-D0CDC0968B50}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{BAD00418-F06A-4B00-923B-8C735A73B583}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BAD00418-F06A-4B00-923B-8C735A73B583}"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
     <sheet name="ESP32" sheetId="2" r:id="rId2"/>
     <sheet name="ESP Board" sheetId="3" r:id="rId3"/>
+    <sheet name="M ctrl" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'ESP Board'!$A$1:$S$24</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>L&amp;K GND</t>
   </si>
@@ -65,18 +66,6 @@
     <t>Buzzer +</t>
   </si>
   <si>
-    <t>TOF VCC</t>
-  </si>
-  <si>
-    <t>TOF GND</t>
-  </si>
-  <si>
-    <t>I2C (TOF+ESP) SDA</t>
-  </si>
-  <si>
-    <t>I2C (TOF+ESP) SCL</t>
-  </si>
-  <si>
     <t>LIDAR VCC</t>
   </si>
   <si>
@@ -89,24 +78,12 @@
     <t>LIDAR UART TXD</t>
   </si>
   <si>
-    <t>ENC_2 A</t>
-  </si>
-  <si>
-    <t>ENC_2 B</t>
-  </si>
-  <si>
     <t>ENC_1 A</t>
   </si>
   <si>
     <t>ENC_1 B</t>
   </si>
   <si>
-    <t>I2C (PI) SDA</t>
-  </si>
-  <si>
-    <t>I2C (PI) SCL</t>
-  </si>
-  <si>
     <t>Servo PWM</t>
   </si>
   <si>
@@ -131,15 +108,9 @@
     <t>ENC_1 GND</t>
   </si>
   <si>
-    <t>ENC_2 GND</t>
-  </si>
-  <si>
     <t>ENC_1 VCC</t>
   </si>
   <si>
-    <t>ENC_2 VCC</t>
-  </si>
-  <si>
     <t>Servo VCC</t>
   </si>
   <si>
@@ -158,7 +129,80 @@
     <t>IMU TXD (SDA)</t>
   </si>
   <si>
-    <t>ESP I2C SDA</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>12V IN</t>
+  </si>
+  <si>
+    <t>GND IN</t>
+  </si>
+  <si>
+    <t>M+</t>
+  </si>
+  <si>
+    <t>M-</t>
+  </si>
+  <si>
+    <t>PI TTL RXD</t>
+  </si>
+  <si>
+    <t>PI TTL TXD</t>
+  </si>
+  <si>
+    <t>ENC_0 VCC</t>
+  </si>
+  <si>
+    <t>ENC_0 A</t>
+  </si>
+  <si>
+    <t>ENC_0 B</t>
+  </si>
+  <si>
+    <t>ENC_0 GND</t>
+  </si>
+  <si>
+    <t>UART (PI) RXD</t>
+  </si>
+  <si>
+    <t>UART (PI) TXD</t>
+  </si>
+  <si>
+    <t>PDU 5V</t>
+  </si>
+  <si>
+    <t>PDU GND</t>
+  </si>
+  <si>
+    <t>(Servo VCC)</t>
+  </si>
+  <si>
+    <t>(SERVO GND)</t>
+  </si>
+  <si>
+    <t>(IMU GND)</t>
+  </si>
+  <si>
+    <t>(ENC1 VCC)</t>
+  </si>
+  <si>
+    <t>(IMU VCC)</t>
+  </si>
+  <si>
+    <t>(IMU PS0)</t>
+  </si>
+  <si>
+    <t>EMERGENCY
+START</t>
+  </si>
+  <si>
+    <t>PSU GND</t>
+  </si>
+  <si>
+    <t>(ENC1 GND)</t>
+  </si>
+  <si>
+    <t>PSU 5V</t>
   </si>
 </sst>
 </file>
@@ -174,7 +218,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,13 +263,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -250,17 +300,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -328,13 +388,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>501649</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>222250</xdr:rowOff>
@@ -422,10 +482,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>109191</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>73454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>81311</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>41704</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{941D118F-1913-666B-F9B7-95B82ECDE398}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1104901" y="614444"/>
+          <a:ext cx="3098800" cy="3121720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 téma">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -463,7 +572,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -569,7 +678,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -711,7 +820,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -725,106 +834,91 @@
   <dimension ref="B1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.81640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.90625" customWidth="1"/>
-    <col min="4" max="4" width="0.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
-    <col min="8" max="8" width="3.90625" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="11"/>
+      <c r="H3" s="5"/>
+      <c r="I3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+    </row>
+    <row r="4" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="6"/>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="H5" s="2"/>
+      <c r="I5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="6" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="4"/>
+      <c r="I6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="5"/>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+    </row>
+    <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="14" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="16" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+    <row r="18" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
+    </row>
+    <row r="21" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
@@ -841,104 +935,164 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B5:I15"/>
+  <dimension ref="A3:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" customWidth="1"/>
-    <col min="3" max="4" width="1.90625" customWidth="1"/>
-    <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" customWidth="1"/>
+    <col min="20" max="20" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="3" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="K3" s="6"/>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="K14" s="1"/>
+      <c r="L14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="H13" s="6"/>
-      <c r="I13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="H14" s="5"/>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="21" spans="3:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -950,152 +1104,174 @@
   </sheetPr>
   <dimension ref="A5:S24"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="4.08984375" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="9" max="10" width="4" customWidth="1"/>
-    <col min="11" max="11" width="7.90625" customWidth="1"/>
-    <col min="17" max="17" width="15.36328125" customWidth="1"/>
-    <col min="18" max="18" width="4.453125" customWidth="1"/>
-    <col min="19" max="19" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="R6" s="9" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="R6" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="S6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B7" s="10"/>
       <c r="R7" s="5"/>
       <c r="S7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
       <c r="R8" s="6"/>
       <c r="S8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="R10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R11" s="2"/>
       <c r="S11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="R13" s="5"/>
       <c r="S13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="R15" s="5"/>
+      <c r="S15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="R17" s="6"/>
+      <c r="S17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="23" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="2"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" ht="144.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J24" s="10" t="s">
-        <v>38</v>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="3"/>
+      <c r="J23" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="151.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1103,4 +1279,99 @@
   <pageSetup paperSize="9" scale="74" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B77D6C1-D557-44FE-93E9-815A1C454C53}">
+  <dimension ref="A3:L25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="22" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="5"/>
+      <c r="L23" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>